<commit_message>
commit v miro uprava excel
</commit_message>
<xml_diff>
--- a/Zošit1.xlsx
+++ b/Zošit1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>OrderDetailID</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:AI519"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +866,9 @@
       <c r="D8" s="6">
         <v>35</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="K8" s="26"/>
       <c r="L8" s="27"/>

</xml_diff>